<commit_message>
Bug fix + Content check
</commit_message>
<xml_diff>
--- a/EnsembleData.xlsx
+++ b/EnsembleData.xlsx
@@ -450,7 +450,7 @@
         <v>Age</v>
       </c>
       <c r="P1" t="str">
-        <v>Shuffle Units</v>
+        <v>Shuffle Units_x000d_</v>
       </c>
     </row>
     <row r="2">
@@ -500,7 +500,7 @@
         <v>18-19</v>
       </c>
       <c r="P2" t="str">
-        <v>Ring.A.Bell</v>
+        <v>Ring.A.Bell_x000d_</v>
       </c>
     </row>
     <row r="3">
@@ -550,7 +550,7 @@
         <v>18-19</v>
       </c>
       <c r="P3" t="str">
-        <v>Puffy*Bunny</v>
+        <v>Puffy*Bunny_x000d_</v>
       </c>
     </row>
     <row r="4">
@@ -600,7 +600,7 @@
         <v>16-17</v>
       </c>
       <c r="P4" t="str">
-        <v>Branco</v>
+        <v>Branco_x000d_</v>
       </c>
     </row>
     <row r="5">
@@ -650,7 +650,7 @@
         <v>17-18</v>
       </c>
       <c r="P5" t="str">
-        <v>Flambe, MVNV</v>
+        <v>Flambe, MVNV_x000d_</v>
       </c>
     </row>
     <row r="6">
@@ -700,7 +700,7 @@
         <v>17-18</v>
       </c>
       <c r="P6" t="str">
-        <v>Getto Spectacle, EVIL NUM+</v>
+        <v>Getto Spectacle, EVIL NUM+_x000d_</v>
       </c>
     </row>
     <row r="7">
@@ -750,7 +750,7 @@
         <v>17-18</v>
       </c>
       <c r="P7" t="str">
-        <v>Flambe</v>
+        <v>Flambe_x000d_</v>
       </c>
     </row>
     <row r="8">
@@ -800,7 +800,7 @@
         <v>17-18</v>
       </c>
       <c r="P8" t="str">
-        <v>XXVeil</v>
+        <v>XXVeil_x000d_</v>
       </c>
     </row>
     <row r="9">
@@ -850,7 +850,7 @@
         <v>17-18</v>
       </c>
       <c r="P9" t="str">
-        <v>Ring.A.Bell</v>
+        <v>Ring.A.Bell_x000d_</v>
       </c>
     </row>
     <row r="10">
@@ -900,7 +900,7 @@
         <v>16-17</v>
       </c>
       <c r="P10" t="str">
-        <v>BUTOUKAI</v>
+        <v>BUTOUKAI_x000d_</v>
       </c>
     </row>
     <row r="11">
@@ -920,7 +920,7 @@
         <v>Orange|Brown</v>
       </c>
       <c r="F11" t="str">
-        <v>Blue</v>
+        <v>Green</v>
       </c>
       <c r="G11" t="str">
         <v>00533F</v>
@@ -950,7 +950,7 @@
         <v>16-17</v>
       </c>
       <c r="P11" t="str">
-        <v>Ring.A.Bell</v>
+        <v>Ring.A.Bell_x000d_</v>
       </c>
     </row>
     <row r="12">
@@ -967,7 +967,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="str">
-        <v>Purple</v>
+        <v>Purple/Yellow</v>
       </c>
       <c r="F12" t="str">
         <v>Orange|Brown</v>
@@ -1000,7 +1000,7 @@
         <v>16-17</v>
       </c>
       <c r="P12" t="str">
-        <v>Puffy*Bunny, Ha/Lo</v>
+        <v>Puffy*Bunny, Ha/Lo_x000d_</v>
       </c>
     </row>
     <row r="13">
@@ -1020,7 +1020,7 @@
         <v>Orange|Brown</v>
       </c>
       <c r="F13" t="str">
-        <v>Orange|Brown</v>
+        <v>Yellow</v>
       </c>
       <c r="G13" t="str">
         <v>E60033</v>
@@ -1050,7 +1050,7 @@
         <v>18-19</v>
       </c>
       <c r="P13" t="str">
-        <v>/AtoZ</v>
+        <v>/AtoZ_x000d_</v>
       </c>
     </row>
     <row r="14">
@@ -1100,7 +1100,7 @@
         <v>18-19</v>
       </c>
       <c r="P14" t="str">
-        <v>Getto Spectacle</v>
+        <v>Getto Spectacle_x000d_</v>
       </c>
     </row>
     <row r="15">
@@ -1150,7 +1150,7 @@
         <v>16-17</v>
       </c>
       <c r="P15" t="str">
-        <v>Puffy*Bunny</v>
+        <v>Puffy*Bunny_x000d_</v>
       </c>
     </row>
     <row r="16">
@@ -1200,7 +1200,7 @@
         <v>15-16</v>
       </c>
       <c r="P16" t="str">
-        <v>Branco</v>
+        <v>Branco_x000d_</v>
       </c>
     </row>
     <row r="17">
@@ -1250,7 +1250,7 @@
         <v>17-18</v>
       </c>
       <c r="P17" t="str">
-        <v>La Mort</v>
+        <v>La Mort_x000d_</v>
       </c>
     </row>
     <row r="18">
@@ -1300,7 +1300,7 @@
         <v>18-19</v>
       </c>
       <c r="P18" t="str">
-        <v>Getto Spectacle</v>
+        <v>Getto Spectacle_x000d_</v>
       </c>
     </row>
     <row r="19">
@@ -1317,7 +1317,7 @@
         <v>Graduated</v>
       </c>
       <c r="E19" t="str">
-        <v>Blond</v>
+        <v>Gray</v>
       </c>
       <c r="F19" t="str">
         <v>Yellow</v>
@@ -1350,7 +1350,7 @@
         <v>18-19</v>
       </c>
       <c r="P19" t="str">
-        <v>La Mort</v>
+        <v>La Mort_x000d_</v>
       </c>
     </row>
     <row r="20">
@@ -1400,7 +1400,7 @@
         <v>18-19</v>
       </c>
       <c r="P20" t="str">
-        <v>Getto Spectacle</v>
+        <v>Getto Spectacle_x000d_</v>
       </c>
     </row>
     <row r="21">
@@ -1450,7 +1450,7 @@
         <v>17-18</v>
       </c>
       <c r="P21" t="str">
-        <v>Flambe</v>
+        <v>Flambe_x000d_</v>
       </c>
     </row>
     <row r="22">
@@ -1500,7 +1500,7 @@
         <v>17-18</v>
       </c>
       <c r="P22" t="str">
-        <v>BUTOUKAI</v>
+        <v>BUTOUKAI_x000d_</v>
       </c>
     </row>
     <row r="23">
@@ -1550,7 +1550,7 @@
         <v>18-19</v>
       </c>
       <c r="P23" t="str">
-        <v>BLEND+</v>
+        <v>BLEND+_x000d_</v>
       </c>
     </row>
     <row r="24">
@@ -1600,7 +1600,7 @@
         <v>17-18</v>
       </c>
       <c r="P24" t="str">
-        <v>Puffy*Bunny</v>
+        <v>Puffy*Bunny_x000d_</v>
       </c>
     </row>
     <row r="25">
@@ -1650,7 +1650,7 @@
         <v>16-17</v>
       </c>
       <c r="P25" t="str">
-        <v>Puffy*Bunny, EVIL NUM+</v>
+        <v>Puffy*Bunny, EVIL NUM+_x000d_</v>
       </c>
     </row>
     <row r="26">
@@ -1700,7 +1700,7 @@
         <v>16-17</v>
       </c>
       <c r="P26" t="str">
-        <v>BLEND+</v>
+        <v>BLEND+_x000d_</v>
       </c>
     </row>
     <row r="27">
@@ -1750,7 +1750,7 @@
         <v>20-21</v>
       </c>
       <c r="P27" t="str">
-        <v>Flambe</v>
+        <v>Flambe_x000d_</v>
       </c>
     </row>
     <row r="28">
@@ -1800,7 +1800,7 @@
         <v>18-19</v>
       </c>
       <c r="P28" t="str">
-        <v>XXVeil</v>
+        <v>XXVeil_x000d_</v>
       </c>
     </row>
     <row r="29">
@@ -1850,7 +1850,7 @@
         <v>15-16</v>
       </c>
       <c r="P29" t="str">
-        <v>La Mort</v>
+        <v>La Mort_x000d_</v>
       </c>
     </row>
     <row r="30">
@@ -1900,7 +1900,7 @@
         <v>18-19</v>
       </c>
       <c r="P30" t="str">
-        <v>/AtoZ, MVNV</v>
+        <v>/AtoZ, MVNV_x000d_</v>
       </c>
     </row>
     <row r="31">
@@ -1920,7 +1920,7 @@
         <v>Black</v>
       </c>
       <c r="F31" t="str">
-        <v>Orange|Brown</v>
+        <v>Red</v>
       </c>
       <c r="G31" t="str">
         <v>47266E</v>
@@ -1950,7 +1950,7 @@
         <v>19-20</v>
       </c>
       <c r="P31" t="str">
-        <v>La Mort, MVNV</v>
+        <v>La Mort, MVNV_x000d_</v>
       </c>
     </row>
     <row r="32">
@@ -2000,7 +2000,7 @@
         <v>18-19</v>
       </c>
       <c r="P32" t="str">
-        <v>/AtoZ</v>
+        <v>/AtoZ_x000d_</v>
       </c>
     </row>
     <row r="33">
@@ -2050,7 +2050,7 @@
         <v>17-18</v>
       </c>
       <c r="P33" t="str">
-        <v>BLEND+</v>
+        <v>BLEND+_x000d_</v>
       </c>
     </row>
     <row r="34">
@@ -2100,7 +2100,7 @@
         <v>17-18</v>
       </c>
       <c r="P34" t="str">
-        <v>BUTOUKAI</v>
+        <v>BUTOUKAI_x000d_</v>
       </c>
     </row>
     <row r="35">
@@ -2150,7 +2150,7 @@
         <v>16-17</v>
       </c>
       <c r="P35" t="str">
-        <v>Flambe, Ha/Lo</v>
+        <v>Flambe, Ha/Lo_x000d_</v>
       </c>
     </row>
     <row r="36">
@@ -2200,7 +2200,7 @@
         <v>18-19</v>
       </c>
       <c r="P36" t="str">
-        <v>XXVeil</v>
+        <v>XXVeil_x000d_</v>
       </c>
     </row>
     <row r="37">
@@ -2250,7 +2250,7 @@
         <v>16-17</v>
       </c>
       <c r="P37" t="str">
-        <v>/AtoZ</v>
+        <v>/AtoZ_x000d_</v>
       </c>
     </row>
     <row r="38">
@@ -2300,7 +2300,7 @@
         <v>16-17</v>
       </c>
       <c r="P38" t="str">
-        <v>Branco, EVIL NUM+</v>
+        <v>Branco, EVIL NUM+_x000d_</v>
       </c>
     </row>
     <row r="39">
@@ -2350,7 +2350,7 @@
         <v>18-19</v>
       </c>
       <c r="P39" t="str">
-        <v>Ring.A.Bell</v>
+        <v>Ring.A.Bell_x000d_</v>
       </c>
     </row>
     <row r="40">
@@ -2400,7 +2400,7 @@
         <v>18-19</v>
       </c>
       <c r="P40" t="str">
-        <v>BUTOUKAI</v>
+        <v>BUTOUKAI_x000d_</v>
       </c>
     </row>
     <row r="41">
@@ -2450,7 +2450,7 @@
         <v>17-18</v>
       </c>
       <c r="P41" t="str">
-        <v>XXVeil</v>
+        <v>XXVeil_x000d_</v>
       </c>
     </row>
     <row r="42">
@@ -2500,7 +2500,7 @@
         <v>16-17</v>
       </c>
       <c r="P42" t="str">
-        <v>BLEND+, Ha/Lo</v>
+        <v>BLEND+, Ha/Lo_x000d_</v>
       </c>
     </row>
     <row r="43">
@@ -2550,7 +2550,7 @@
         <v>18-19</v>
       </c>
       <c r="P43" t="str">
-        <v>Ring.A.Bell</v>
+        <v>Ring.A.Bell_x000d_</v>
       </c>
     </row>
     <row r="44">
@@ -2600,7 +2600,7 @@
         <v>18-19</v>
       </c>
       <c r="P44" t="str">
-        <v>XXVeil</v>
+        <v>XXVeil_x000d_</v>
       </c>
     </row>
     <row r="45">
@@ -2620,7 +2620,7 @@
         <v>Black</v>
       </c>
       <c r="F45" t="str">
-        <v>Orange|Brown</v>
+        <v>Red</v>
       </c>
       <c r="G45" t="str">
         <v>001E43</v>
@@ -2650,7 +2650,7 @@
         <v>18-19</v>
       </c>
       <c r="P45" t="str">
-        <v>La Mort, EVIL NUM+</v>
+        <v>La Mort, EVIL NUM+_x000d_</v>
       </c>
     </row>
     <row r="46">
@@ -2700,7 +2700,7 @@
         <v>17-18</v>
       </c>
       <c r="P46" t="str">
-        <v>Getto Spectacle</v>
+        <v>Getto Spectacle_x000d_</v>
       </c>
     </row>
     <row r="47">
@@ -2717,7 +2717,7 @@
         <v>3</v>
       </c>
       <c r="E47" t="str">
-        <v>Red|Maroon</v>
+        <v>Red|Maroon/Gray</v>
       </c>
       <c r="F47" t="str">
         <v>Yellow</v>
@@ -2750,7 +2750,7 @@
         <v>17-18</v>
       </c>
       <c r="P47" t="str">
-        <v>/AtoZ, EVIL NUM+</v>
+        <v>/AtoZ, EVIL NUM+_x000d_</v>
       </c>
     </row>
     <row r="48">
@@ -2800,7 +2800,7 @@
         <v>18-19</v>
       </c>
       <c r="P48" t="str">
-        <v>BLEND+, MVNV</v>
+        <v>BLEND+, MVNV_x000d_</v>
       </c>
     </row>
     <row r="49">
@@ -2817,7 +2817,7 @@
         <v>2</v>
       </c>
       <c r="E49" t="str">
-        <v>Blond</v>
+        <v>Blond/Green</v>
       </c>
       <c r="F49" t="str">
         <v>Blue</v>
@@ -2850,7 +2850,7 @@
         <v>16-17</v>
       </c>
       <c r="P49" t="str">
-        <v>Branco</v>
+        <v>Branco_x000d_</v>
       </c>
     </row>
     <row r="50">

</xml_diff>

<commit_message>
Akatsuki.png please I am begging you
</commit_message>
<xml_diff>
--- a/EnsembleData.xlsx
+++ b/EnsembleData.xlsx
@@ -2311,7 +2311,7 @@
         <v>Rhythm Link</v>
       </c>
       <c r="C39" t="str">
-        <v>AKATSUKI</v>
+        <v>Akatsuki</v>
       </c>
       <c r="D39" t="str">
         <v>Graduated</v>
@@ -2361,7 +2361,7 @@
         <v>Rhythm Link</v>
       </c>
       <c r="C40" t="str">
-        <v>AKATSUKI</v>
+        <v>Akatsuki</v>
       </c>
       <c r="D40" t="str">
         <v>Graduated</v>
@@ -2411,7 +2411,7 @@
         <v>Rhythm Link</v>
       </c>
       <c r="C41" t="str">
-        <v>AKATSUKI</v>
+        <v>Akatsuki</v>
       </c>
       <c r="D41" t="str">
         <v>3</v>

</xml_diff>